<commit_message>
refactor: screenshot, add comments, names change
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/ReadData.xlsx
+++ b/src/test/assets/exceldocuments/ReadData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="113">
   <si>
     <t xml:space="preserve">IP</t>
   </si>
@@ -88,7 +88,7 @@
     <t xml:space="preserve">Cantón</t>
   </si>
   <si>
-    <t xml:space="preserve">Parroquía</t>
+    <t xml:space="preserve">Parroquia</t>
   </si>
   <si>
     <t xml:space="preserve">¿Aplica Preajuste?</t>
@@ -97,7 +97,7 @@
     <t xml:space="preserve">Forma de Pago</t>
   </si>
   <si>
-    <t xml:space="preserve">Debito Cuenta</t>
+    <t xml:space="preserve">Débito Cuenta</t>
   </si>
   <si>
     <t xml:space="preserve">Comentario</t>
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Análisis de Crédito</t>
   </si>
   <si>
-    <t xml:space="preserve">Abono o cancelacion</t>
+    <t xml:space="preserve">Abono o cancelación</t>
   </si>
   <si>
     <t xml:space="preserve">Observaciones</t>
@@ -166,7 +166,7 @@
     <t xml:space="preserve">Buzón de Autorizaciones</t>
   </si>
   <si>
-    <t xml:space="preserve">Transacción</t>
+    <t xml:space="preserve">Transacción Aprobadora</t>
   </si>
   <si>
     <t xml:space="preserve">Aprobación de Análisis de Riesgos</t>
@@ -193,19 +193,22 @@
     <t xml:space="preserve">Número Garantía</t>
   </si>
   <si>
-    <t xml:space="preserve">Emision de documentos habilitantes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Transaccion</t>
+    <t xml:space="preserve">Emisión de Documentos Habilitantes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validación Documentos de Crédito</t>
   </si>
   <si>
     <t xml:space="preserve">Estatus</t>
   </si>
   <si>
-    <t xml:space="preserve">Credito a Cuentas -Cuenta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verificar desembolso</t>
+    <t xml:space="preserve">Forma de Desembolso del Préstamo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crédito a Cuentas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verificar Desembolso</t>
   </si>
   <si>
     <t xml:space="preserve">10.16.5.64</t>
@@ -510,11 +513,11 @@
   </sheetPr>
   <dimension ref="A1:BP6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="BG1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="BO2" activeCellId="0" sqref="BO2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
@@ -544,6 +547,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="13.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="14.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="10.58"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="45" min="45" style="0" width="13.57"/>
@@ -552,6 +556,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="0" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="60" min="60" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="62" min="62" style="0" width="15.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="0" width="14.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="0" width="13.75"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -741,7 +747,7 @@
       <c r="BJ1" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="BK1" s="0" t="s">
+      <c r="BK1" s="4" t="s">
         <v>58</v>
       </c>
       <c r="BL1" s="1" t="s">
@@ -750,220 +756,220 @@
       <c r="BM1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="BN1" s="0" t="s">
-        <v>58</v>
+      <c r="BN1" s="4" t="s">
+        <v>60</v>
       </c>
       <c r="BO1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="BP1" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="R2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="S2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB2" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="J2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="R2" s="6" t="s">
-        <v>79</v>
-      </c>
-      <c r="S2" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="T2" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="U2" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="V2" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="W2" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="Y2" s="8" t="s">
+      <c r="AC2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG2" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH2" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI2" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ2" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK2" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL2" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM2" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="Z2" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="AA2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AN2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP2" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AV2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AX2" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AY2" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="AD2" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AE2" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF2" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="AG2" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="AH2" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="AK2" s="6" t="s">
+      <c r="AZ2" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="BA2" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="AL2" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="AM2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AN2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AO2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AP2" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="AQ2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AR2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AS2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AT2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AU2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AV2" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="AW2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="AX2" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="AY2" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="AZ2" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="BA2" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="BB2" s="6" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="BC2" s="6" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="BD2" s="9" t="n">
         <v>2001</v>
       </c>
       <c r="BE2" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="BF2" s="8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="BG2" s="8" t="n">
         <v>3000407614</v>
       </c>
       <c r="BH2" s="8" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="BI2" s="8" t="n">
         <v>90000157848</v>
       </c>
       <c r="BJ2" s="8" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="BK2" s="0" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="BL2" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="BM2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="BN2" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="BO2" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="BN2" s="0" t="s">
-        <v>110</v>
-      </c>
-      <c r="BO2" s="9" t="s">
-        <v>87</v>
-      </c>
       <c r="BP2" s="0" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
feat: refactor loanflow tr063002v3
</commit_message>
<xml_diff>
--- a/src/test/assets/exceldocuments/ReadData.xlsx
+++ b/src/test/assets/exceldocuments/ReadData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="115">
   <si>
     <t xml:space="preserve">IP</t>
   </si>
@@ -359,6 +359,12 @@
   </si>
   <si>
     <t xml:space="preserve">06-4022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0190082847001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BA01001212</t>
   </si>
 </sst>
 </file>
@@ -514,10 +520,10 @@
   <dimension ref="A1:BP6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.43"/>
@@ -972,7 +978,418 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P3" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q3" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="S3" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="T3" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="U3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="V3" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="W3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="X3" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y3" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC3" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE3" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL3" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP3" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AV3" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW3" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AX3" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AY3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ3" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="BA3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB3" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC3" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="BD3" s="9" t="n">
+        <v>2001</v>
+      </c>
+      <c r="BE3" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="BF3" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG3" s="8" t="n">
+        <v>3000407614</v>
+      </c>
+      <c r="BH3" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="BI3" s="8" t="n">
+        <v>90000157848</v>
+      </c>
+      <c r="BJ3" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="BK3" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="BL3" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="BM3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="BN3" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="BO3" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="BP3" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="N4" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="S4" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="U4" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="V4" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="W4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y4" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z4" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AB4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="AC4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD4" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF4" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="AG4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="AH4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="AI4" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="AJ4" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="AK4" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="AL4" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="AM4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AN4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AO4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AP4" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="AQ4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AR4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AS4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AT4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AV4" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="AW4" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="AX4" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="AY4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ4" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="BA4" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB4" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="BC4" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="BD4" s="9" t="n">
+        <v>2001</v>
+      </c>
+      <c r="BE4" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="BF4" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="BG4" s="8" t="n">
+        <v>3000407614</v>
+      </c>
+      <c r="BH4" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="BI4" s="8" t="n">
+        <v>90000157848</v>
+      </c>
+      <c r="BJ4" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="BK4" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="BL4" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="BM4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="BN4" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="BO4" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="BP4" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>